<commit_message>
Actualización Procedimiento Reporte PTU
</commit_message>
<xml_diff>
--- a/senosiain/horas-quincena 2 Abri 2025.xlsx
+++ b/senosiain/horas-quincena 2 Abri 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Terceros\fortia\senosiain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F02585-B2C9-49A0-8E6A-F969F2938D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE7B9E8-8C5F-4CFF-8F13-7B7165910839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>fecha</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>2da Quincena Abril 2025</t>
+  </si>
+  <si>
+    <t>Meet de Revisión de Proceso de cambio de contraseña</t>
+  </si>
+  <si>
+    <t>Generación de procedimiento para reseteo de la contraseña de usuarios adam-</t>
   </si>
 </sst>
 </file>
@@ -495,7 +501,7 @@
   <dimension ref="A1:H994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -571,18 +577,26 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
+      <c r="A5" s="12">
+        <v>45782</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12"/>
@@ -768,7 +782,7 @@
       </c>
       <c r="D33" s="10">
         <f>SUBTOTAL(109,D3:D32)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E33" s="1"/>
     </row>
@@ -776,7 +790,7 @@
     <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D35" s="19">
         <f>+D33*500</f>
-        <v>1500</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -800,7 +814,7 @@
       </c>
       <c r="D39" s="20">
         <f>+D35-D37</f>
-        <v>1500</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>